<commit_message>
Format precision data Insert precision data into excel sheet Update overall data
</commit_message>
<xml_diff>
--- a/data/overall.xlsx
+++ b/data/overall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/floh/Code/sgx-benchmark/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30DA4349-0517-D446-BC44-F59034769744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F3CC13-2890-4246-82A8-B0AE278E1A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21500" yWindow="2260" windowWidth="27640" windowHeight="16860" xr2:uid="{5EB75DF4-15B7-3B47-94ED-3A0DBF8788E7}"/>
   </bookViews>
@@ -261,7 +261,7 @@
                   <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -599,7 +599,7 @@
                   <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -937,7 +937,7 @@
                   <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.21</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1275,7 +1275,7 @@
                   <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.46</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1613,7 +1613,7 @@
                   <c:v>13.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5.42</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1951,13 +1951,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>54.46</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18.559999999999999</c:v>
+                  <c:v>18.600000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2393,22 +2393,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.21</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.46</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>5.42</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>54.46</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2592,7 +2592,7 @@
                   <c:v>1.88</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18.559999999999999</c:v>
+                  <c:v>18.600000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3047,16 +3047,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.21</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.46</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8319,7 +8319,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8375,22 +8375,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>0.21</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.46</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>5.42</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>54.46</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -8436,7 +8436,7 @@
         <v>1.88</v>
       </c>
       <c r="G5">
-        <v>18.559999999999999</v>
+        <v>18.600000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Insert data for 10 GB of ice lake cpu Remove raw data from precision Update overall and readme
</commit_message>
<xml_diff>
--- a/data/overall.xlsx
+++ b/data/overall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/floh/Code/sgx-benchmark/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F3CC13-2890-4246-82A8-B0AE278E1A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D8B64C-3FAD-1747-B24E-BD69E281F907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21500" yWindow="2260" windowWidth="27640" windowHeight="16860" xr2:uid="{5EB75DF4-15B7-3B47-94ED-3A0DBF8788E7}"/>
   </bookViews>
@@ -1957,7 +1957,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18.600000000000001</c:v>
+                  <c:v>18.64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2592,7 +2592,7 @@
                   <c:v>1.88</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18.600000000000001</c:v>
+                  <c:v>18.64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3342,6 +3342,647 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1912495408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Overall &lt;= 1 GB</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pentium Silver J5005</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Tabelle1!$B$1:$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1 MB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10 MB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80 MB</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100 MB</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1 GB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$2:$F$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-967E-F240-9F3E-30D8D5C1A08A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Xeon W-10885M</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Tabelle1!$B$1:$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1 MB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10 MB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80 MB</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100 MB</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1 GB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$3:$F$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.42</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-967E-F240-9F3E-30D8D5C1A08A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Xeon E5-2666G</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Tabelle1!$B$1:$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1 MB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10 MB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80 MB</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100 MB</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1 GB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$4:$F$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-967E-F240-9F3E-30D8D5C1A08A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Xeon Gold 5315Y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Tabelle1!$B$1:$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1 MB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10 MB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80 MB</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100 MB</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1 GB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$5:$F$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.88</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-967E-F240-9F3E-30D8D5C1A08A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1945366448"/>
+        <c:axId val="1945368096"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1945366448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1945368096"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1945368096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1945366448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3758,6 +4399,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="222">
   <cs:axisTitle>
@@ -7231,6 +7912,502 @@
 </file>
 
 <file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8016,6 +9193,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>146050</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E1828CE-9256-0F48-96FC-2FABF2F19BF1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8318,9 +9531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5053F5-BE28-FD41-8714-82D129A695D1}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8436,7 +9647,7 @@
         <v>1.88</v>
       </c>
       <c r="G5">
-        <v>18.600000000000001</v>
+        <v>18.64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Insert data for hp proliant Update reamde Insert diagrams for <= 1 GB enclaves
</commit_message>
<xml_diff>
--- a/data/overall.xlsx
+++ b/data/overall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/floh/Code/sgx-benchmark/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D8B64C-3FAD-1747-B24E-BD69E281F907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38FA9784-5331-C64F-9D04-A25A801ECCDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21500" yWindow="2260" windowWidth="27640" windowHeight="16860" xr2:uid="{5EB75DF4-15B7-3B47-94ED-3A0DBF8788E7}"/>
   </bookViews>
@@ -264,7 +264,7 @@
                   <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.01</c:v>
@@ -602,7 +602,7 @@
                   <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.03</c:v>
@@ -940,7 +940,7 @@
                   <c:v>0.21</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.18</c:v>
@@ -1278,7 +1278,7 @@
                   <c:v>0.46</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.22</c:v>
@@ -1616,7 +1616,7 @@
                   <c:v>5.42</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>5.31</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.88</c:v>
@@ -1954,7 +1954,7 @@
                   <c:v>54.46</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>18.64</c:v>
@@ -2485,22 +2485,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>5.31</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3127,16 +3127,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3759,19 +3759,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>5.31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9531,7 +9531,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5053F5-BE28-FD41-8714-82D129A695D1}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9609,22 +9611,22 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>5.31</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update precision 10 GB data set Update readme Clean up raw data
</commit_message>
<xml_diff>
--- a/data/overall.xlsx
+++ b/data/overall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/floh/Code/sgx-benchmark/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38FA9784-5331-C64F-9D04-A25A801ECCDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194FF9FF-A493-1345-8168-26CB8C8AFF0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21500" yWindow="2260" windowWidth="27640" windowHeight="16860" xr2:uid="{5EB75DF4-15B7-3B47-94ED-3A0DBF8788E7}"/>
   </bookViews>
@@ -1951,7 +1951,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>54.46</c:v>
+                  <c:v>54.67</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>53</c:v>
@@ -2408,7 +2408,7 @@
                   <c:v>5.42</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>54.46</c:v>
+                  <c:v>54.67</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9532,7 +9532,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9603,7 +9603,7 @@
         <v>5.42</v>
       </c>
       <c r="G3">
-        <v>54.46</v>
+        <v>54.67</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Insert diagrams for overall
</commit_message>
<xml_diff>
--- a/data/overall.xlsx
+++ b/data/overall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/floh/Code/sgx-benchmark/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194FF9FF-A493-1345-8168-26CB8C8AFF0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3BD1C1D-04E7-4944-BF28-1BFE864BF29B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21500" yWindow="2260" windowWidth="27640" windowHeight="16860" xr2:uid="{5EB75DF4-15B7-3B47-94ED-3A0DBF8788E7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Pentium Silver J5005</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>Xeon E5-2666G</t>
-  </si>
-  <si>
-    <t>Not enough memory.</t>
   </si>
 </sst>
 </file>
@@ -1923,19 +1920,16 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$A$2:$A$5</c:f>
+              <c:f>Tabelle1!$A$3:$A$5</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Pentium Silver J5005</c:v>
+                  <c:v>Xeon W-10885M</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Xeon W-10885M</c:v>
+                  <c:v>Xeon E5-2666G</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Xeon E5-2666G</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>Xeon Gold 5315Y</c:v>
                 </c:pt>
               </c:strCache>
@@ -1943,20 +1937,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$G$2:$G$5</c:f>
+              <c:f>Tabelle1!$G$3:$G$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>54.67</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>54.67</c:v>
+                  <c:v>53.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>18.64</c:v>
                 </c:pt>
               </c:numCache>
@@ -2316,7 +2307,7 @@
                   <c:v>13.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>3420</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2500,7 +2491,7 @@
                   <c:v>5.31</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>53</c:v>
+                  <c:v>53.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9129,10 +9120,10 @@
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9531,8 +9522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5053F5-BE28-FD41-8714-82D129A695D1}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G67" sqref="G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9579,8 +9570,8 @@
       <c r="F2">
         <v>13.25</v>
       </c>
-      <c r="G2" t="s">
-        <v>10</v>
+      <c r="G2">
+        <v>3420</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -9626,7 +9617,7 @@
         <v>5.31</v>
       </c>
       <c r="G4">
-        <v>53</v>
+        <v>53.5</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fix cpu name in diagrams
</commit_message>
<xml_diff>
--- a/data/overall.xlsx
+++ b/data/overall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/floh/Code/sgx-benchmark/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3BD1C1D-04E7-4944-BF28-1BFE864BF29B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9BA8689-1A86-F84A-9424-282F8BF89906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21500" yWindow="2260" windowWidth="27640" windowHeight="16860" xr2:uid="{5EB75DF4-15B7-3B47-94ED-3A0DBF8788E7}"/>
   </bookViews>
@@ -63,7 +63,7 @@
     <t>10 GB</t>
   </si>
   <si>
-    <t>Xeon E5-2666G</t>
+    <t>Xeon E5-2276G</t>
   </si>
 </sst>
 </file>
@@ -240,7 +240,7 @@
                   <c:v>Xeon W-10885M</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Xeon E5-2666G</c:v>
+                  <c:v>Xeon E5-2276G</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Xeon Gold 5315Y</c:v>
@@ -578,7 +578,7 @@
                   <c:v>Xeon W-10885M</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Xeon E5-2666G</c:v>
+                  <c:v>Xeon E5-2276G</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Xeon Gold 5315Y</c:v>
@@ -916,7 +916,7 @@
                   <c:v>Xeon W-10885M</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Xeon E5-2666G</c:v>
+                  <c:v>Xeon E5-2276G</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Xeon Gold 5315Y</c:v>
@@ -1254,7 +1254,7 @@
                   <c:v>Xeon W-10885M</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Xeon E5-2666G</c:v>
+                  <c:v>Xeon E5-2276G</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Xeon Gold 5315Y</c:v>
@@ -1592,7 +1592,7 @@
                   <c:v>Xeon W-10885M</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Xeon E5-2666G</c:v>
+                  <c:v>Xeon E5-2276G</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Xeon Gold 5315Y</c:v>
@@ -1927,7 +1927,7 @@
                   <c:v>Xeon W-10885M</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Xeon E5-2666G</c:v>
+                  <c:v>Xeon E5-2276G</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Xeon Gold 5315Y</c:v>
@@ -2420,7 +2420,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Xeon E5-2666G</c:v>
+                  <c:v>Xeon E5-2276G</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3068,7 +3068,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Xeon E5-2666G</c:v>
+                  <c:v>Xeon E5-2276G</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3697,7 +3697,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Xeon E5-2666G</c:v>
+                  <c:v>Xeon E5-2276G</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -9522,8 +9522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5053F5-BE28-FD41-8714-82D129A695D1}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G67" sqref="G67"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Insert 10 GB data for hp proliant server Update small amount of values
</commit_message>
<xml_diff>
--- a/data/overall.xlsx
+++ b/data/overall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/floh/Code/sgx-benchmark/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949A3CC3-0235-E54F-83B3-C58449F8C342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E175D6-93CF-3542-B97C-C0E965230C99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21500" yWindow="2260" windowWidth="27640" windowHeight="16860" xr2:uid="{5EB75DF4-15B7-3B47-94ED-3A0DBF8788E7}"/>
   </bookViews>
@@ -1945,7 +1945,7 @@
                   <c:v>54.67</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>53.5</c:v>
+                  <c:v>53.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>18.64</c:v>
@@ -2491,7 +2491,7 @@
                   <c:v>5.31</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>53.5</c:v>
+                  <c:v>53.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9522,8 +9522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5053F5-BE28-FD41-8714-82D129A695D1}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9617,7 +9617,7 @@
         <v>5.31</v>
       </c>
       <c r="G4">
-        <v>53.5</v>
+        <v>53.6</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>